<commit_message>
add tests for 0.64
</commit_message>
<xml_diff>
--- a/test/perl_output/chart_pie.xlsx
+++ b/test/perl_output/chart_pie.xlsx
@@ -180,6 +180,125 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pie Chart with user defined colors</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pie sales data</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="5ABA10"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FE110E"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="CA5C05"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Apple</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cherry</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pecan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -207,6 +326,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>

</xml_diff>